<commit_message>
implement basic calculation for cars and public_transport
</commit_message>
<xml_diff>
--- a/CO2_data.xlsx
+++ b/CO2_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Horea\Project_Green_Maps_CO2_CalculatorProject_Green_Maps_CO2_Calculator\carbon-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C2E50C-0F01-4ABA-84F3-D26F0C4F5E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4386C5-B11D-4EF1-AC71-D076C9AD8CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{3404CFC5-9E90-4505-9000-1946D4220711}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Cars" sheetId="1" r:id="rId1"/>
+    <sheet name="Public_transport" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
   <si>
     <t>Diesel</t>
   </si>
@@ -170,13 +170,22 @@
     <t>Average car</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>C1</t>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>0.105</t>
+  </si>
+  <si>
+    <t>Railway</t>
+  </si>
+  <si>
+    <t>0.041</t>
+  </si>
+  <si>
+    <t>Transport_type</t>
+  </si>
+  <si>
+    <t>kg CO2e/km</t>
   </si>
 </sst>
 </file>
@@ -776,11 +785,11 @@
     <xf numFmtId="165" fontId="18" fillId="0" borderId="9" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="30" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="40" borderId="9" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="30" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="18" fillId="0" borderId="9" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1147,7 +1156,7 @@
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1160,54 +1169,54 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12" t="s">
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
       <c r="P1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12" t="s">
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12" t="s">
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12" t="s">
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
@@ -1317,10 +1326,10 @@
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1408,8 +1417,8 @@
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1495,8 +1504,8 @@
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1600,8 +1609,8 @@
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1703,8 +1712,8 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1808,8 +1817,8 @@
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1911,8 +1920,8 @@
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -2016,8 +2025,8 @@
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2120,11 +2129,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="T1:W1"/>
     <mergeCell ref="X1:AA1"/>
@@ -2133,6 +2137,11 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="P1:S1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2140,39 +2149,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3388C464-863B-4430-8514-1BC688D3CCD0}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>